<commit_message>
finally, all converted with proper columns
</commit_message>
<xml_diff>
--- a/Data from Paho/excels/2014/excel/2014-Sep-19---CHA--CHIKV--cases-EW-40.xlsx
+++ b/Data from Paho/excels/2014/excel/2014-Sep-19---CHA--CHIKV--cases-EW-40.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\chikonguniya\Data from Paho\excels\2014\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E2310ADB-1534-40AC-A024-12ED075C7979}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="19230" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="150">
   <si>
     <t>Country/Territory</t>
   </si>
@@ -253,9 +259,6 @@
     <t>Week 19</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>Autochthonous transmission casesb</t>
   </si>
   <si>
@@ -338,9 +341,6 @@
   </si>
   <si>
     <t>1,415</t>
-  </si>
-  <si>
-    <t>Incidence Rate</t>
   </si>
   <si>
     <t>4,675.0</t>
@@ -475,8 +475,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,6 +513,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -559,7 +567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,9 +599,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -625,6 +651,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -800,26 +844,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="2" max="8" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -829,1351 +867,1345 @@
       <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
-        <v>80</v>
+      <c r="E1" t="s">
+        <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
         <v>118</v>
       </c>
-      <c r="J1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>61</v>
       </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
       <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="D8">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="E11">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>16</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
       </c>
-      <c r="D12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12">
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12">
         <v>54</v>
       </c>
+      <c r="F12">
+        <v>259.39999999999998</v>
+      </c>
       <c r="G12">
-        <v>259.4</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="E13">
+      <c r="D13">
         <v>8</v>
       </c>
-      <c r="H13">
+      <c r="F13">
         <v>0.1</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F15">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
       </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
       <c r="E16">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F16">
-        <v>17</v>
-      </c>
-      <c r="H16">
         <v>0.3</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
-        <v>82</v>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17">
+        <v>73</v>
       </c>
       <c r="E17">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="F17">
-        <v>55</v>
+        <v>36.5</v>
       </c>
       <c r="G17">
-        <v>36.5</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
       <c r="E19">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F19">
-        <v>13</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20">
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20">
         <v>84</v>
       </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20">
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20">
         <v>6</v>
       </c>
-      <c r="J20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="H20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>61</v>
       </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
       <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
+        <v>96</v>
+      </c>
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22">
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22">
         <v>430</v>
       </c>
-      <c r="G22" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22">
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22">
         <v>49</v>
       </c>
-      <c r="J22">
+      <c r="H22">
         <v>466</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23">
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23">
         <v>14</v>
       </c>
+      <c r="F23">
+        <v>627.20000000000005</v>
+      </c>
       <c r="G23">
-        <v>627.2</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
       <c r="D24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" t="s">
-        <v>112</v>
-      </c>
-      <c r="I24">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24">
         <v>56</v>
       </c>
-      <c r="J24">
+      <c r="H24">
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>66</v>
       </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
       <c r="D25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="E25">
+        <v>25</v>
       </c>
       <c r="F25">
-        <v>25</v>
+        <v>256.10000000000002</v>
       </c>
       <c r="G25">
-        <v>256.1</v>
-      </c>
-      <c r="I25">
         <v>3</v>
       </c>
-      <c r="J25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="H25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
+      <c r="C26">
+        <v>985</v>
+      </c>
       <c r="D26">
-        <v>985</v>
-      </c>
-      <c r="E26">
         <v>142</v>
       </c>
-      <c r="G26" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
+      <c r="F26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="D27" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27">
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27">
         <v>793</v>
       </c>
-      <c r="G27" t="s">
-        <v>114</v>
-      </c>
-      <c r="I27">
+      <c r="F27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27">
         <v>3</v>
       </c>
-      <c r="J27">
+      <c r="H27">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
       <c r="D28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28">
+        <v>99</v>
+      </c>
+      <c r="E28">
         <v>38</v>
       </c>
-      <c r="G28" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28">
+      <c r="F28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28">
         <v>117</v>
       </c>
-      <c r="J28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="H28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="E30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="s">
-        <v>91</v>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31">
+        <v>78</v>
       </c>
       <c r="E31">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F31">
-        <v>7</v>
-      </c>
-      <c r="H31">
         <v>10</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
       <c r="E33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
       <c r="B34" t="s">
         <v>61</v>
       </c>
+      <c r="C34">
+        <v>841</v>
+      </c>
       <c r="D34">
-        <v>841</v>
+        <v>328</v>
       </c>
       <c r="E34">
-        <v>328</v>
+        <v>70</v>
       </c>
       <c r="F34">
-        <v>70</v>
-      </c>
-      <c r="H34">
         <v>4</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
-        <v>92</v>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35">
+        <v>406</v>
       </c>
       <c r="E35">
-        <v>406</v>
+        <v>83</v>
       </c>
       <c r="F35">
-        <v>83</v>
-      </c>
-      <c r="H35">
         <v>4</v>
       </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
       </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
       <c r="E37">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F37">
-        <v>7</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>61</v>
       </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
       <c r="E38">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="F38">
-        <v>36</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>68</v>
       </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="E39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>69</v>
       </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
       <c r="E40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
       <c r="D41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="F41">
-        <v>46</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>70</v>
       </c>
+      <c r="D43">
+        <v>38</v>
+      </c>
       <c r="E43">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>237.5</v>
       </c>
       <c r="G43">
-        <v>237.5</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="H43">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
         <v>71</v>
       </c>
+      <c r="C44">
+        <v>679</v>
+      </c>
       <c r="D44">
-        <v>679</v>
-      </c>
-      <c r="E44">
         <v>18</v>
       </c>
+      <c r="F44">
+        <v>774.4</v>
+      </c>
       <c r="G44">
-        <v>774.4</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="H44">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>63</v>
       </c>
+      <c r="C45">
+        <v>85</v>
+      </c>
       <c r="D45">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="E45">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F45">
-        <v>12</v>
+        <v>95.4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>95.4</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>72</v>
       </c>
+      <c r="D46">
+        <v>79</v>
+      </c>
       <c r="E46">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
       </c>
       <c r="H46">
-        <v>21</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>63</v>
       </c>
+      <c r="C47">
+        <v>77</v>
+      </c>
       <c r="D47">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F47">
-        <v>8</v>
+        <v>27.7</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>27.7</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
         <v>289</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
       <c r="B48" t="s">
         <v>71</v>
       </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
       <c r="E48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>1.9</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>1.9</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
       </c>
+      <c r="C49">
+        <v>607</v>
+      </c>
       <c r="D49">
-        <v>607</v>
+        <v>58</v>
       </c>
       <c r="E49">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="F49">
-        <v>7</v>
+        <v>452.4</v>
       </c>
       <c r="G49">
-        <v>452.4</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="H49">
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>44</v>
       </c>
       <c r="B50" t="s">
         <v>65</v>
       </c>
-      <c r="D50" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50">
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50">
         <v>141</v>
       </c>
-      <c r="G50" t="s">
-        <v>116</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
+      <c r="F50" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
       <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="E51">
+      <c r="D51">
         <v>5</v>
       </c>
+      <c r="F51">
+        <v>4.5</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
       <c r="H51">
-        <v>4.5</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-      <c r="J51">
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
       <c r="B52" t="s">
         <v>70</v>
       </c>
-      <c r="E52">
+      <c r="D52">
         <v>76</v>
       </c>
+      <c r="F52">
+        <v>9.5</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
       <c r="H52">
-        <v>9.5</v>
-      </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-      <c r="J52">
         <v>800</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
       <c r="B53" t="s">
         <v>74</v>
       </c>
+      <c r="C53">
+        <v>194</v>
+      </c>
       <c r="D53">
-        <v>194</v>
+        <v>28</v>
       </c>
       <c r="E53">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F53">
-        <v>3</v>
-      </c>
-      <c r="H53">
         <v>8</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="J53" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="E54">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
         <v>0</v>
       </c>
       <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-      <c r="J54">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
       <c r="B55" t="s">
         <v>75</v>
       </c>
+      <c r="C55">
+        <v>31</v>
+      </c>
       <c r="D55">
-        <v>31</v>
-      </c>
-      <c r="E55">
         <v>28</v>
       </c>
+      <c r="F55">
+        <v>115.7</v>
+      </c>
       <c r="G55">
-        <v>115.7</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>50</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
+      <c r="C56">
+        <v>214</v>
+      </c>
       <c r="D56">
-        <v>214</v>
-      </c>
-      <c r="E56">
         <v>120</v>
       </c>
+      <c r="F56">
+        <v>204.9</v>
+      </c>
       <c r="G56">
-        <v>204.9</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="H56">
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
       <c r="B57" t="s">
         <v>76</v>
       </c>
+      <c r="C57">
+        <v>329</v>
+      </c>
       <c r="D57">
-        <v>329</v>
-      </c>
-      <c r="E57">
         <v>67</v>
       </c>
+      <c r="F57">
+        <v>384.5</v>
+      </c>
       <c r="G57">
-        <v>384.5</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="H57">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
       <c r="B58" t="s">
         <v>77</v>
       </c>
-      <c r="E58">
+      <c r="D58">
         <v>360</v>
       </c>
+      <c r="F58">
+        <v>900</v>
+      </c>
       <c r="G58">
-        <v>900</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="H58">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
       <c r="B59" t="s">
         <v>61</v>
       </c>
+      <c r="D59">
+        <v>594</v>
+      </c>
       <c r="E59">
-        <v>594</v>
+        <v>14</v>
       </c>
       <c r="F59">
-        <v>14</v>
+        <v>110.2</v>
       </c>
       <c r="G59">
-        <v>110.2</v>
-      </c>
-      <c r="I59">
         <v>1</v>
       </c>
-      <c r="J59">
+      <c r="H59">
         <v>539</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>54</v>
       </c>
       <c r="B60" t="s">
         <v>72</v>
       </c>
+      <c r="D60">
+        <v>43</v>
+      </c>
       <c r="E60">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="F60">
-        <v>3</v>
-      </c>
-      <c r="H60">
         <v>3.2</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
       </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
       <c r="E61">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F61">
-        <v>7</v>
+        <v>20.8</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>20.8</v>
-      </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-      <c r="J61">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>56</v>
       </c>
       <c r="B62" t="s">
         <v>78</v>
       </c>
-      <c r="E62">
+      <c r="D62">
         <v>20</v>
       </c>
+      <c r="F62">
+        <v>62.5</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
       <c r="H62">
-        <v>62.5</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
       <c r="B63" t="s">
         <v>72</v>
       </c>
+      <c r="C63">
+        <v>728</v>
+      </c>
       <c r="D63">
-        <v>728</v>
+        <v>51</v>
       </c>
       <c r="E63">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>741.9</v>
       </c>
       <c r="G63">
-        <v>741.9</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="H63">
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
       <c r="D64" t="s">
-        <v>94</v>
-      </c>
-      <c r="E64" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="E64">
+        <v>65</v>
       </c>
       <c r="F64">
-        <v>65</v>
+        <v>113.6</v>
       </c>
       <c r="G64">
-        <v>113.6</v>
-      </c>
-      <c r="I64">
         <v>1</v>
       </c>
-      <c r="J64" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="H64" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>58</v>
       </c>
+      <c r="C65" t="s">
+        <v>94</v>
+      </c>
       <c r="D65" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E65" t="s">
-        <v>102</v>
-      </c>
-      <c r="F65" t="s">
-        <v>107</v>
-      </c>
-      <c r="H65">
+        <v>106</v>
+      </c>
+      <c r="F65">
         <v>77.5</v>
       </c>
-      <c r="I65">
+      <c r="G65">
         <v>118</v>
       </c>
-      <c r="J65" t="s">
-        <v>151</v>
+      <c r="H65" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>